<commit_message>
Coreccion de plantilla de correo para invalidacion
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_tiempo_personal.xlsx
+++ b/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_tiempo_personal.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_retenciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED31112-7C85-4A42-B317-9823F0731309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95109D9-D1EF-4199-82F9-DEB348E62AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71471483-0F7B-4877-9266-78025D47BF67}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tiempo Personal" sheetId="1" r:id="rId1"/>
     <sheet name="Tipos" sheetId="2" r:id="rId2"/>
     <sheet name="Estado" sheetId="3" r:id="rId3"/>
+    <sheet name="Empresas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Descripción</t>
   </si>
@@ -72,6 +73,18 @@
   </si>
   <si>
     <t>Estado del recibo de nómina</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>AE DE PAZ</t>
+  </si>
+  <si>
+    <t>INNUFFE</t>
+  </si>
+  <si>
+    <t>INVERSIONES COMERCIALES ESCOBAR SA DE CV</t>
   </si>
 </sst>
 </file>
@@ -106,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -114,11 +127,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -130,6 +182,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,117 +499,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E21E8D-BFAF-4274-A0B3-B7B382542769}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="37.69140625" customWidth="1"/>
-    <col min="3" max="3" width="30.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.07421875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.69140625" customWidth="1"/>
+    <col min="4" max="4" width="30.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.07421875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D671EAB-FB56-4C99-B4E0-BE95A92340D7}">
           <x14:formula1>
             <xm:f>Tipos!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AD89BA5-924B-4688-9655-200C0D2CA4F7}">
           <x14:formula1>
             <xm:f>Estado!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{135371B0-76C7-4C5D-8547-3ADAA08BB472}">
+          <x14:formula1>
+            <xm:f>Empresas!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -610,12 +684,13 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
@@ -641,4 +716,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED59037-B58C-4287-A5BC-E9E960DF75CA}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="40.765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>